<commit_message>
Třídní diagram a relační datový model
</commit_message>
<xml_diff>
--- a/Working sheet for database model.xlsx
+++ b/Working sheet for database model.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>settings</t>
   </si>
@@ -669,7 +669,7 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,6 +729,9 @@
       <c r="D3" t="s">
         <v>74</v>
       </c>
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
@@ -988,9 +991,6 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="H14" s="8" t="s">
         <v>11</v>
       </c>
@@ -999,9 +999,6 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="I15" s="6" t="s">
         <v>32</v>
       </c>
@@ -1036,5 +1033,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>